<commit_message>
Updates to run mission sims
Updates to the routes Excel. Also adds slurm file to run HC_Operations_LA
</commit_message>
<xml_diff>
--- a/03_Aircraft_Noise_Modeling/City_Simulations/Los_Angeles/UAM_City_Routes.xlsx
+++ b/03_Aircraft_Noise_Modeling/City_Simulations/Los_Angeles/UAM_City_Routes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidanmolloy/Documents/LEADS/RESEARCH/03_Aircraft_Noise_Modeling/City_Simulations/Los_Angeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9B6597-17AA-F249-A6D0-19D9A52DED75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC15290-6509-754B-B545-03D3FB545E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="4800" windowWidth="22040" windowHeight="14840" xr2:uid="{0D3479EF-2BF9-A044-90EB-A477301D535B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{0D3479EF-2BF9-A044-90EB-A477301D535B}"/>
   </bookViews>
   <sheets>
     <sheet name="Los_Angeles" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="48">
   <si>
     <t>Origin Code</t>
   </si>
@@ -157,9 +157,6 @@
     <t>LAEP</t>
   </si>
   <si>
-    <t>−118.236944</t>
-  </si>
-  <si>
     <t>USC South park Center (PPR Heliport)</t>
   </si>
   <si>
@@ -176,39 +173,6 @@
   </si>
   <si>
     <t>LAWC</t>
-  </si>
-  <si>
-    <t>−118.236945</t>
-  </si>
-  <si>
-    <t>−118.236946</t>
-  </si>
-  <si>
-    <t>−118.236947</t>
-  </si>
-  <si>
-    <t>−118.236948</t>
-  </si>
-  <si>
-    <t>−118.236950</t>
-  </si>
-  <si>
-    <t>−118.236951</t>
-  </si>
-  <si>
-    <t>−118.236953</t>
-  </si>
-  <si>
-    <t>−118.236955</t>
-  </si>
-  <si>
-    <t>−118.236956</t>
-  </si>
-  <si>
-    <t>−118.236959</t>
-  </si>
-  <si>
-    <t>−118.236962</t>
   </si>
   <si>
     <t>Origin Latitude</t>
@@ -715,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25855B7F-4EAB-EE45-B3D7-2264B8DE67FE}">
   <dimension ref="A1:L201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.2"/>
@@ -740,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -758,7 +722,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>8</v>
@@ -767,7 +731,7 @@
         <v>14</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" x14ac:dyDescent="0.2">
@@ -1219,10 +1183,10 @@
         <v>260</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="I13" s="14">
         <v>34.039496999999997</v>
@@ -1258,10 +1222,10 @@
         <v>260</v>
       </c>
       <c r="G14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I14" s="14">
         <v>33.950713999999998</v>
@@ -1297,10 +1261,10 @@
         <v>260</v>
       </c>
       <c r="G15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I15" s="11">
         <v>34.180481999999998</v>
@@ -1734,8 +1698,8 @@
       <c r="I26" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J26" s="10" t="s">
-        <v>39</v>
+      <c r="J26" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K26" s="12">
         <v>223</v>
@@ -1765,10 +1729,10 @@
         <v>260</v>
       </c>
       <c r="G27" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="I27" s="14">
         <v>34.039496999999997</v>
@@ -1804,10 +1768,10 @@
         <v>260</v>
       </c>
       <c r="G28" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I28" s="14">
         <v>33.950713999999998</v>
@@ -1843,10 +1807,10 @@
         <v>260</v>
       </c>
       <c r="G29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I29" s="11">
         <v>34.180481999999998</v>
@@ -2280,8 +2244,8 @@
       <c r="I40" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J40" s="10" t="s">
-        <v>39</v>
+      <c r="J40" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K40" s="12">
         <v>223</v>
@@ -2311,10 +2275,10 @@
         <v>240</v>
       </c>
       <c r="G41" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H41" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="I41" s="14">
         <v>34.039496999999997</v>
@@ -2350,10 +2314,10 @@
         <v>240</v>
       </c>
       <c r="G42" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I42" s="11">
         <v>34.180481999999998</v>
@@ -2787,8 +2751,8 @@
       <c r="I53" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J53" s="10" t="s">
-        <v>39</v>
+      <c r="J53" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K53" s="12">
         <v>223</v>
@@ -2818,10 +2782,10 @@
         <v>300</v>
       </c>
       <c r="G54" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H54" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="I54" s="14">
         <v>34.039496999999997</v>
@@ -2857,10 +2821,10 @@
         <v>300</v>
       </c>
       <c r="G55" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H55" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I55" s="14">
         <v>33.950713999999998</v>
@@ -2896,10 +2860,10 @@
         <v>300</v>
       </c>
       <c r="G56" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H56" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I56" s="11">
         <v>34.180481999999998</v>
@@ -3333,8 +3297,8 @@
       <c r="I67" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J67" s="10" t="s">
-        <v>39</v>
+      <c r="J67" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K67" s="12">
         <v>223</v>
@@ -3364,10 +3328,10 @@
         <v>200</v>
       </c>
       <c r="G68" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H68" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="H68" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="I68" s="14">
         <v>34.039496999999997</v>
@@ -3403,10 +3367,10 @@
         <v>200</v>
       </c>
       <c r="G69" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H69" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H69" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I69" s="14">
         <v>33.950713999999998</v>
@@ -3442,10 +3406,10 @@
         <v>200</v>
       </c>
       <c r="G70" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H70" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I70" s="11">
         <v>34.180481999999998</v>
@@ -3879,8 +3843,8 @@
       <c r="I81" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J81" s="10" t="s">
-        <v>39</v>
+      <c r="J81" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K81" s="12">
         <v>223</v>
@@ -3910,10 +3874,10 @@
         <v>230</v>
       </c>
       <c r="G82" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H82" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="H82" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="I82" s="14">
         <v>34.039496999999997</v>
@@ -3949,10 +3913,10 @@
         <v>230</v>
       </c>
       <c r="G83" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H83" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H83" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I83" s="14">
         <v>33.950713999999998</v>
@@ -3988,10 +3952,10 @@
         <v>230</v>
       </c>
       <c r="G84" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H84" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H84" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I84" s="11">
         <v>34.180481999999998</v>
@@ -4425,8 +4389,8 @@
       <c r="I95" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J95" s="10" t="s">
-        <v>39</v>
+      <c r="J95" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K95" s="12">
         <v>223</v>
@@ -4456,10 +4420,10 @@
         <v>210</v>
       </c>
       <c r="G96" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H96" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="H96" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="I96" s="14">
         <v>34.039496999999997</v>
@@ -4495,10 +4459,10 @@
         <v>210</v>
       </c>
       <c r="G97" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H97" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H97" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I97" s="14">
         <v>33.950713999999998</v>
@@ -4534,10 +4498,10 @@
         <v>210</v>
       </c>
       <c r="G98" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H98" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H98" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I98" s="11">
         <v>34.180481999999998</v>
@@ -4971,8 +4935,8 @@
       <c r="I109" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J109" s="10" t="s">
-        <v>39</v>
+      <c r="J109" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K109" s="12">
         <v>223</v>
@@ -5002,10 +4966,10 @@
         <v>230</v>
       </c>
       <c r="G110" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H110" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="H110" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="I110" s="14">
         <v>34.039496999999997</v>
@@ -5041,10 +5005,10 @@
         <v>230</v>
       </c>
       <c r="G111" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H111" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H111" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I111" s="14">
         <v>33.950713999999998</v>
@@ -5080,10 +5044,10 @@
         <v>230</v>
       </c>
       <c r="G112" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H112" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H112" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I112" s="11">
         <v>34.180481999999998</v>
@@ -5509,10 +5473,10 @@
         <v>230</v>
       </c>
       <c r="G123" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H123" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H123" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I123" s="14">
         <v>33.950713999999998</v>
@@ -5548,10 +5512,10 @@
         <v>230</v>
       </c>
       <c r="G124" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H124" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H124" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I124" s="11">
         <v>34.180481999999998</v>
@@ -5985,8 +5949,8 @@
       <c r="I135" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J135" s="10" t="s">
-        <v>39</v>
+      <c r="J135" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K135" s="12">
         <v>223</v>
@@ -6016,10 +5980,10 @@
         <v>250</v>
       </c>
       <c r="G136" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H136" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="H136" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="I136" s="14">
         <v>34.039496999999997</v>
@@ -6055,10 +6019,10 @@
         <v>250</v>
       </c>
       <c r="G137" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H137" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H137" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I137" s="11">
         <v>34.180481999999998</v>
@@ -6492,8 +6456,8 @@
       <c r="I148" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J148" s="10" t="s">
-        <v>39</v>
+      <c r="J148" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K148" s="12">
         <v>223</v>
@@ -6523,10 +6487,10 @@
         <v>160</v>
       </c>
       <c r="G149" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H149" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="H149" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="I149" s="14">
         <v>34.039496999999997</v>
@@ -6562,10 +6526,10 @@
         <v>160</v>
       </c>
       <c r="G150" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H150" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H150" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I150" s="14">
         <v>33.950713999999998</v>
@@ -6601,10 +6565,10 @@
         <v>160</v>
       </c>
       <c r="G151" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H151" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H151" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I151" s="11">
         <v>34.180481999999998</v>
@@ -6630,8 +6594,8 @@
       <c r="C152" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="D152" s="10" t="s">
-        <v>39</v>
+      <c r="D152" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E152" s="12">
         <v>223</v>
@@ -6669,8 +6633,8 @@
       <c r="C153" s="10">
         <v>35.082777999999998</v>
       </c>
-      <c r="D153" s="10" t="s">
-        <v>46</v>
+      <c r="D153" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E153" s="12">
         <v>224</v>
@@ -6708,8 +6672,8 @@
       <c r="C154" s="10">
         <v>36.082777999999998</v>
       </c>
-      <c r="D154" s="10" t="s">
-        <v>47</v>
+      <c r="D154" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E154" s="12">
         <v>225</v>
@@ -6747,8 +6711,8 @@
       <c r="C155" s="10">
         <v>37.082777999999998</v>
       </c>
-      <c r="D155" s="10" t="s">
-        <v>48</v>
+      <c r="D155" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E155" s="12">
         <v>226</v>
@@ -6786,8 +6750,8 @@
       <c r="C156" s="10">
         <v>38.082777999999998</v>
       </c>
-      <c r="D156" s="10" t="s">
-        <v>49</v>
+      <c r="D156" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E156" s="12">
         <v>227</v>
@@ -6825,8 +6789,8 @@
       <c r="C157" s="10">
         <v>40.082777999999998</v>
       </c>
-      <c r="D157" s="10" t="s">
-        <v>50</v>
+      <c r="D157" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E157" s="12">
         <v>229</v>
@@ -6864,8 +6828,8 @@
       <c r="C158" s="10">
         <v>41.082777999999998</v>
       </c>
-      <c r="D158" s="10" t="s">
-        <v>51</v>
+      <c r="D158" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E158" s="12">
         <v>230</v>
@@ -6903,8 +6867,8 @@
       <c r="C159" s="10">
         <v>43.082777999999998</v>
       </c>
-      <c r="D159" s="10" t="s">
-        <v>52</v>
+      <c r="D159" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E159" s="12">
         <v>232</v>
@@ -6942,8 +6906,8 @@
       <c r="C160" s="10">
         <v>45.082777999999998</v>
       </c>
-      <c r="D160" s="10" t="s">
-        <v>53</v>
+      <c r="D160" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E160" s="12">
         <v>234</v>
@@ -6981,8 +6945,8 @@
       <c r="C161" s="10">
         <v>46.082777999999998</v>
       </c>
-      <c r="D161" s="10" t="s">
-        <v>54</v>
+      <c r="D161" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E161" s="12">
         <v>235</v>
@@ -7020,8 +6984,8 @@
       <c r="C162" s="10">
         <v>49.082777999999998</v>
       </c>
-      <c r="D162" s="10" t="s">
-        <v>55</v>
+      <c r="D162" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E162" s="12">
         <v>238</v>
@@ -7030,10 +6994,10 @@
         <v>230</v>
       </c>
       <c r="G162" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H162" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H162" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I162" s="14">
         <v>33.950713999999998</v>
@@ -7059,8 +7023,8 @@
       <c r="C163" s="10">
         <v>52.082777999999998</v>
       </c>
-      <c r="D163" s="10" t="s">
-        <v>56</v>
+      <c r="D163" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="E163" s="12">
         <v>241</v>
@@ -7069,10 +7033,10 @@
         <v>230</v>
       </c>
       <c r="G163" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H163" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H163" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I163" s="11">
         <v>34.180481999999998</v>
@@ -7090,10 +7054,10 @@
     </row>
     <row r="164" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A164" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B164" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B164" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C164" s="14">
         <v>34.039496999999997</v>
@@ -7129,10 +7093,10 @@
     </row>
     <row r="165" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A165" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B165" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B165" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C165" s="14">
         <v>34.039496999999997</v>
@@ -7168,10 +7132,10 @@
     </row>
     <row r="166" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A166" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B166" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B166" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C166" s="14">
         <v>34.039496999999997</v>
@@ -7207,10 +7171,10 @@
     </row>
     <row r="167" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A167" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B167" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B167" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C167" s="14">
         <v>34.039496999999997</v>
@@ -7246,10 +7210,10 @@
     </row>
     <row r="168" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A168" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B168" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C168" s="14">
         <v>34.039496999999997</v>
@@ -7285,10 +7249,10 @@
     </row>
     <row r="169" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A169" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B169" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B169" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C169" s="14">
         <v>34.039496999999997</v>
@@ -7324,10 +7288,10 @@
     </row>
     <row r="170" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A170" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B170" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B170" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C170" s="14">
         <v>34.039496999999997</v>
@@ -7363,10 +7327,10 @@
     </row>
     <row r="171" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A171" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B171" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B171" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C171" s="14">
         <v>34.039496999999997</v>
@@ -7402,10 +7366,10 @@
     </row>
     <row r="172" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A172" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B172" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B172" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C172" s="14">
         <v>34.039496999999997</v>
@@ -7441,10 +7405,10 @@
     </row>
     <row r="173" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A173" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B173" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B173" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C173" s="14">
         <v>34.039496999999997</v>
@@ -7480,10 +7444,10 @@
     </row>
     <row r="174" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A174" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B174" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B174" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C174" s="14">
         <v>34.039496999999997</v>
@@ -7498,10 +7462,10 @@
         <v>230</v>
       </c>
       <c r="G174" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H174" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H174" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I174" s="14">
         <v>33.950713999999998</v>
@@ -7519,10 +7483,10 @@
     </row>
     <row r="175" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A175" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B175" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B175" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C175" s="14">
         <v>34.039496999999997</v>
@@ -7537,10 +7501,10 @@
         <v>230</v>
       </c>
       <c r="G175" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H175" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H175" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I175" s="11">
         <v>34.180481999999998</v>
@@ -7558,10 +7522,10 @@
     </row>
     <row r="176" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A176" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B176" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B176" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C176" s="14">
         <v>33.950713999999998</v>
@@ -7597,10 +7561,10 @@
     </row>
     <row r="177" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A177" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B177" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B177" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C177" s="14">
         <v>33.950713999999998</v>
@@ -7636,10 +7600,10 @@
     </row>
     <row r="178" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A178" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B178" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B178" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C178" s="14">
         <v>33.950713999999998</v>
@@ -7675,10 +7639,10 @@
     </row>
     <row r="179" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A179" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B179" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B179" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C179" s="14">
         <v>33.950713999999998</v>
@@ -7714,10 +7678,10 @@
     </row>
     <row r="180" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A180" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B180" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B180" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C180" s="14">
         <v>33.950713999999998</v>
@@ -7753,10 +7717,10 @@
     </row>
     <row r="181" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A181" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B181" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B181" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C181" s="14">
         <v>33.950713999999998</v>
@@ -7792,10 +7756,10 @@
     </row>
     <row r="182" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A182" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B182" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B182" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C182" s="14">
         <v>33.950713999999998</v>
@@ -7831,10 +7795,10 @@
     </row>
     <row r="183" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A183" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B183" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B183" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C183" s="14">
         <v>33.950713999999998</v>
@@ -7870,10 +7834,10 @@
     </row>
     <row r="184" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A184" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B184" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B184" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C184" s="14">
         <v>33.950713999999998</v>
@@ -7909,10 +7873,10 @@
     </row>
     <row r="185" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A185" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B185" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B185" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C185" s="14">
         <v>33.950713999999998</v>
@@ -7948,10 +7912,10 @@
     </row>
     <row r="186" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A186" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B186" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B186" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C186" s="14">
         <v>33.950713999999998</v>
@@ -7974,8 +7938,8 @@
       <c r="I186" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J186" s="10" t="s">
-        <v>39</v>
+      <c r="J186" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K186" s="12">
         <v>223</v>
@@ -7987,10 +7951,10 @@
     </row>
     <row r="187" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A187" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B187" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B187" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C187" s="14">
         <v>33.950713999999998</v>
@@ -8005,10 +7969,10 @@
         <v>230</v>
       </c>
       <c r="G187" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H187" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="H187" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="I187" s="14">
         <v>34.039496999999997</v>
@@ -8026,10 +7990,10 @@
     </row>
     <row r="188" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A188" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B188" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B188" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C188" s="14">
         <v>33.950713999999998</v>
@@ -8044,10 +8008,10 @@
         <v>230</v>
       </c>
       <c r="G188" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H188" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H188" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="I188" s="11">
         <v>34.180481999999998</v>
@@ -8065,10 +8029,10 @@
     </row>
     <row r="189" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A189" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B189" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B189" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C189" s="11">
         <v>34.180481999999998</v>
@@ -8104,10 +8068,10 @@
     </row>
     <row r="190" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A190" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B190" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B190" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C190" s="11">
         <v>34.180481999999998</v>
@@ -8143,10 +8107,10 @@
     </row>
     <row r="191" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A191" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B191" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B191" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C191" s="11">
         <v>34.180481999999998</v>
@@ -8182,10 +8146,10 @@
     </row>
     <row r="192" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A192" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B192" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B192" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C192" s="11">
         <v>34.180481999999998</v>
@@ -8221,10 +8185,10 @@
     </row>
     <row r="193" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A193" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B193" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B193" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C193" s="11">
         <v>34.180481999999998</v>
@@ -8260,10 +8224,10 @@
     </row>
     <row r="194" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A194" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B194" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B194" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C194" s="11">
         <v>34.180481999999998</v>
@@ -8299,10 +8263,10 @@
     </row>
     <row r="195" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A195" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B195" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B195" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C195" s="11">
         <v>34.180481999999998</v>
@@ -8338,10 +8302,10 @@
     </row>
     <row r="196" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A196" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B196" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B196" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C196" s="11">
         <v>34.180481999999998</v>
@@ -8377,10 +8341,10 @@
     </row>
     <row r="197" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A197" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B197" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B197" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C197" s="11">
         <v>34.180481999999998</v>
@@ -8416,10 +8380,10 @@
     </row>
     <row r="198" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A198" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B198" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C198" s="11">
         <v>34.180481999999998</v>
@@ -8455,10 +8419,10 @@
     </row>
     <row r="199" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A199" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B199" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B199" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C199" s="11">
         <v>34.180481999999998</v>
@@ -8481,8 +8445,8 @@
       <c r="I199" s="10">
         <v>34.082777999999998</v>
       </c>
-      <c r="J199" s="10" t="s">
-        <v>39</v>
+      <c r="J199" s="10">
+        <v>-118.23690000000001</v>
       </c>
       <c r="K199" s="12">
         <v>223</v>
@@ -8494,10 +8458,10 @@
     </row>
     <row r="200" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A200" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B200" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B200" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C200" s="11">
         <v>34.180481999999998</v>
@@ -8512,10 +8476,10 @@
         <v>230</v>
       </c>
       <c r="G200" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H200" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="H200" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="I200" s="14">
         <v>34.039496999999997</v>
@@ -8533,10 +8497,10 @@
     </row>
     <row r="201" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A201" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B201" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B201" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C201" s="11">
         <v>34.180481999999998</v>
@@ -8551,10 +8515,10 @@
         <v>230</v>
       </c>
       <c r="G201" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H201" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H201" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="I201" s="14">
         <v>33.950713999999998</v>

</xml_diff>